<commit_message>
Update safeguarding config (#77)
Co-authored-by: Ian Stride <ianstride@gmail.com>
</commit_message>
<xml_diff>
--- a/excel_files/safeguarding chinese.xlsx
+++ b/excel_files/safeguarding chinese.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmun\Code\parenttext-china\excel_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fagio\Documents\GitHub\parenttext-china\excel_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA365AB-DD40-416A-8E50-A3D6C69D5A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A807189-8100-4B8A-AD75-80902D149FBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-480" windowWidth="29040" windowHeight="15720" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="9" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="generic" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1320" uniqueCount="949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="948">
   <si>
     <t>Section 1</t>
   </si>
@@ -2875,9 +2875,6 @@
     <t>站厅</t>
   </si>
   <si>
-    <t>停</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
@@ -2899,17 +2896,17 @@
     <t>上课</t>
   </si>
   <si>
-    <t>上客</t>
-  </si>
-  <si>
-    <t>上科</t>
+    <t>余北学</t>
+  </si>
+  <si>
+    <t>余北师</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2958,6 +2955,13 @@
       <sz val="12"/>
       <color rgb="FF3F3F42"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -3182,7 +3186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3218,6 +3222,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -3239,7 +3244,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3475,19 +3480,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -3507,20 +3512,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -3542,20 +3547,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -3574,19 +3579,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -11424,19 +11429,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>915</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -11456,20 +11461,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -11491,20 +11496,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -11523,19 +11528,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -13396,7 +13401,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F5" sqref="F5:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13412,19 +13417,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>916</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -13444,20 +13449,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -13479,20 +13484,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -13511,19 +13516,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -13557,9 +13562,7 @@
       <c r="E5" s="5" t="s">
         <v>934</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>534</v>
-      </c>
+      <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -13598,9 +13601,7 @@
       <c r="E6" s="5" t="s">
         <v>938</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>939</v>
-      </c>
+      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -15404,19 +15405,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>534</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -15436,20 +15437,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -15471,20 +15472,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -15503,19 +15504,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -15538,7 +15539,7 @@
         <v>130</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -15571,16 +15572,16 @@
         <v>535</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>942</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>943</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>944</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>945</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -17370,7 +17371,7 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17386,19 +17387,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>940</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>939</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -17418,20 +17419,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -17453,20 +17454,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -17485,19 +17486,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -17520,7 +17521,7 @@
         <v>130</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
@@ -17553,17 +17554,15 @@
         <v>535</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>945</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>946</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>947</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>948</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>948</v>
-      </c>
+      <c r="E6" s="5"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -19343,7 +19342,7 @@
     <mergeCell ref="F3:K3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -19368,19 +19367,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -19400,20 +19399,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -19435,20 +19434,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -19467,19 +19466,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -22024,19 +22023,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -22056,20 +22055,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -22091,20 +22090,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -22123,19 +22122,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -24212,19 +24211,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -24244,20 +24243,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -24279,20 +24278,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -24311,19 +24310,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -28209,7 +28208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AA1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -28226,19 +28225,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>513</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -28258,20 +28257,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -28293,20 +28292,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -28325,19 +28324,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -30222,19 +30221,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>507</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -30254,20 +30253,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -30289,20 +30288,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -30321,19 +30320,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -32210,19 +32209,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>533</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -32242,20 +32241,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -32277,20 +32276,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -32309,19 +32308,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -34200,19 +34199,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>520</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -34232,20 +34231,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -34267,20 +34266,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -34299,19 +34298,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
@@ -36192,19 +36191,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="33" t="s">
         <v>914</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="34"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="35"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -36224,20 +36223,20 @@
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="35" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
-      <c r="K2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="32"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -36259,20 +36258,20 @@
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="37" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="32"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -36291,19 +36290,19 @@
       <c r="AA3" s="1"/>
     </row>
     <row r="4" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>

</xml_diff>